<commit_message>
Making th first row frozen
</commit_message>
<xml_diff>
--- a/met-api/src/met_api/generated_documents_carbone_templates/proponent_comments_sheet.xlsx
+++ b/met-api/src/met_api/generated_documents_carbone_templates/proponent_comments_sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27130"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{742846CF-FA6E-437D-87AD-52859AE05C49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCAE06BA-8B51-4893-8BE1-302AE6EBB5E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -351,7 +351,8 @@
   <dimension ref="A1:O1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="12.75"/>

</xml_diff>